<commit_message>
actualiza dashboard y graficos
</commit_message>
<xml_diff>
--- a/assets/tabulados/Auditoria_fina.xlsx
+++ b/assets/tabulados/Auditoria_fina.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t xml:space="preserve">encuesta</t>
   </si>
@@ -50,7 +50,7 @@
     <t xml:space="preserve">Verificación</t>
   </si>
   <si>
-    <t xml:space="preserve">CamiloR_ELE</t>
+    <t xml:space="preserve">CamiloR</t>
   </si>
   <si>
     <t xml:space="preserve">25</t>
@@ -65,7 +65,7 @@
     <t xml:space="preserve">16,00</t>
   </si>
   <si>
-    <t xml:space="preserve">CatalinaJ_ELE</t>
+    <t xml:space="preserve">CatalinaJ</t>
   </si>
   <si>
     <t xml:space="preserve">7</t>
@@ -77,7 +77,7 @@
     <t xml:space="preserve">28,57</t>
   </si>
   <si>
-    <t xml:space="preserve">HoracioM_ELE</t>
+    <t xml:space="preserve">HoracioM</t>
   </si>
   <si>
     <t xml:space="preserve">30</t>
@@ -86,7 +86,7 @@
     <t xml:space="preserve">3,33</t>
   </si>
   <si>
-    <t xml:space="preserve">RodolfoV_ELE</t>
+    <t xml:space="preserve">RodolfoV</t>
   </si>
   <si>
     <t xml:space="preserve">17</t>
@@ -95,7 +95,7 @@
     <t xml:space="preserve">52,94</t>
   </si>
   <si>
-    <t xml:space="preserve">ThiareM_ELE</t>
+    <t xml:space="preserve">ThiareM</t>
   </si>
   <si>
     <t xml:space="preserve">15</t>
@@ -110,9 +110,6 @@
     <t xml:space="preserve">Consistencia</t>
   </si>
   <si>
-    <t xml:space="preserve">CatalinaJ_ENI</t>
-  </si>
-  <si>
     <t xml:space="preserve">686</t>
   </si>
   <si>
@@ -122,16 +119,13 @@
     <t xml:space="preserve">4,08</t>
   </si>
   <si>
-    <t xml:space="preserve">HoracioM_ENI</t>
-  </si>
-  <si>
     <t xml:space="preserve">497</t>
   </si>
   <si>
     <t xml:space="preserve">1,01</t>
   </si>
   <si>
-    <t xml:space="preserve">MarcelaP_EOC</t>
+    <t xml:space="preserve">MarcelaP</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
@@ -140,9 +134,6 @@
     <t xml:space="preserve">100,00</t>
   </si>
   <si>
-    <t xml:space="preserve">RodolfoV_ENI</t>
-  </si>
-  <si>
     <t xml:space="preserve">33</t>
   </si>
   <si>
@@ -152,9 +143,6 @@
     <t xml:space="preserve">21,21</t>
   </si>
   <si>
-    <t xml:space="preserve">ThiareM_ENI</t>
-  </si>
-  <si>
     <t xml:space="preserve">190</t>
   </si>
   <si>
@@ -218,7 +206,7 @@
     <t xml:space="preserve">ENIA</t>
   </si>
   <si>
-    <t xml:space="preserve">CristianG_ENIA</t>
+    <t xml:space="preserve">CristianG</t>
   </si>
   <si>
     <t xml:space="preserve">1.028</t>
@@ -233,7 +221,7 @@
     <t xml:space="preserve">28,79</t>
   </si>
   <si>
-    <t xml:space="preserve">DanielaV_ENIA</t>
+    <t xml:space="preserve">DanielaV</t>
   </si>
   <si>
     <t xml:space="preserve">61</t>
@@ -246,9 +234,6 @@
   </si>
   <si>
     <t xml:space="preserve">32,79</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MarcelaP_ENIA</t>
   </si>
   <si>
     <t xml:space="preserve">308</t>
@@ -819,10 +804,10 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -834,13 +819,13 @@
         <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" t="n">
         <v>28</v>
       </c>
       <c r="J7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
@@ -851,10 +836,10 @@
         <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -866,13 +851,13 @@
         <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I8" t="n">
         <v>5</v>
       </c>
       <c r="J8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9">
@@ -883,16 +868,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -915,10 +900,10 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -930,13 +915,13 @@
         <v>5</v>
       </c>
       <c r="H10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I10" t="n">
         <v>7</v>
       </c>
       <c r="J10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
@@ -947,10 +932,10 @@
         <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -962,13 +947,13 @@
         <v>15</v>
       </c>
       <c r="H11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I11" t="n">
         <v>52</v>
       </c>
       <c r="J11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12">
@@ -976,13 +961,13 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -994,13 +979,13 @@
         <v>1036</v>
       </c>
       <c r="H12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I12" t="n">
         <v>7</v>
       </c>
       <c r="J12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13">
@@ -1008,13 +993,13 @@
         <v>30</v>
       </c>
       <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
         <v>50</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" t="s">
-        <v>54</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -1026,13 +1011,13 @@
         <v>277</v>
       </c>
       <c r="H13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I13" t="n">
         <v>3</v>
       </c>
       <c r="J13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14">
@@ -1040,10 +1025,10 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
         <v>28</v>
@@ -1064,7 +1049,7 @@
         <v>4</v>
       </c>
       <c r="J14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15">
@@ -1072,13 +1057,13 @@
         <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -1090,13 +1075,13 @@
         <v>10</v>
       </c>
       <c r="H15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I15" t="n">
         <v>12</v>
       </c>
       <c r="J15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16">
@@ -1107,10 +1092,10 @@
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -1122,13 +1107,13 @@
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I16" t="n">
         <v>8</v>
       </c>
       <c r="J16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17">
@@ -1139,10 +1124,10 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -1154,91 +1139,91 @@
         <v>2</v>
       </c>
       <c r="H17" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I17" t="n">
         <v>4</v>
       </c>
       <c r="J17" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
         <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E18" t="n">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G18" t="n">
         <v>290</v>
       </c>
       <c r="H18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I18" t="n">
         <v>296</v>
       </c>
       <c r="J18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
         <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G19" t="n">
         <v>14</v>
       </c>
       <c r="H19" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I19" t="n">
         <v>20</v>
       </c>
       <c r="J19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
         <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -1250,59 +1235,59 @@
         <v>99</v>
       </c>
       <c r="H20" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="I20" t="n">
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E21" t="n">
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G21" t="n">
         <v>105</v>
       </c>
       <c r="H21" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="I21" t="n">
         <v>304</v>
       </c>
       <c r="J21" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D22" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -1314,27 +1299,27 @@
         <v>13</v>
       </c>
       <c r="H22" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="I22" t="n">
         <v>92</v>
       </c>
       <c r="J22" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -1352,7 +1337,7 @@
         <v>13</v>
       </c>
       <c r="J23" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>